<commit_message>
Moved Images and Forum Page
</commit_message>
<xml_diff>
--- a/Docs/Datasets/MRA.xlsx
+++ b/Docs/Datasets/MRA.xlsx
@@ -16,18 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
-    <t>MPA Name</t>
-  </si>
-  <si>
-    <t>Longitude (E)</t>
-  </si>
-  <si>
-    <t>Latitude (N)</t>
-  </si>
-  <si>
-    <t>Area (km²)</t>
-  </si>
-  <si>
     <t>State/UT</t>
   </si>
   <si>
@@ -206,6 +194,18 @@
   </si>
   <si>
     <t>72.60-72.70</t>
+  </si>
+  <si>
+    <t>MPA_Name</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Area</t>
   </si>
 </sst>
 </file>
@@ -462,383 +462,383 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>260</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>340</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>577.26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1">
         <v>842.5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1">
         <v>4.5999999999999996</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1">
         <v>89.97</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1">
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1">
         <v>209.31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1">
         <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1">
         <v>61.52</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1">
         <v>14.66</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D13" s="1">
         <v>33.25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1">
         <v>4.33</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D15" s="1">
         <v>4.33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1">
         <v>4.33</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1">
         <v>4.33</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1">
         <v>4.33</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1">
         <v>4.33</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1">
         <v>4.33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1">
         <v>4.33</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1">
         <v>4.3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>